<commit_message>
Testing input and expected files now match properly
</commit_message>
<xml_diff>
--- a/tests/integration_test/testing_files/Teacher Two.xlsx
+++ b/tests/integration_test/testing_files/Teacher Two.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan.oldford/Documents/Programming/cycle_calendar_generator/tests/integration_test/testing_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6392FDF6-D6B2-5F48-A2DF-2FF8365D066E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35A0191-EAD6-7C4F-9F94-67F6B41C7732}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17440" xr2:uid="{ADCDD068-B7EC-234E-983D-64D9DE4E15DC}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Excel files now use User Schedule instead of Teacher Schedule as sheet name, since not just teachers could use this
</commit_message>
<xml_diff>
--- a/tests/integration_test/testing_files/Teacher Two.xlsx
+++ b/tests/integration_test/testing_files/Teacher Two.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan.oldford/Documents/Programming/cycle_calendar_generator/tests/integration_test/testing_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35A0191-EAD6-7C4F-9F94-67F6B41C7732}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CB08F0-0C9B-604B-8DA3-718ACBE7FCA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17440" xr2:uid="{ADCDD068-B7EC-234E-983D-64D9DE4E15DC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Teacher Schedule" sheetId="1" r:id="rId1"/>
+    <sheet name="User Schedule" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>

</xml_diff>